<commit_message>
Support imports from any SynBioHub instance whose URL starts with "https://synbiohub" Also add an additional test for exporting
</commit_message>
<xml_diff>
--- a/package template.xlsx
+++ b/package template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557C0736-C2E0-1446-A4EC-3BDBFC7E0354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAD901-DE52-FF44-8A54-8328496CED01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="800" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7547" uniqueCount="7517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7552" uniqueCount="7521">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22645,6 +22645,18 @@
   </si>
   <si>
     <t>Literal Part</t>
+  </si>
+  <si>
+    <t>SynBioHub</t>
+  </si>
+  <si>
+    <t>https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/LmrA/1</t>
+  </si>
+  <si>
+    <t>SynBioHub: https://synbiohub.programmingbiology.org/public/Eco1C1G1T1/LmrA/1</t>
+  </si>
+  <si>
+    <t>{REPLACE_HERE}</t>
   </si>
 </sst>
 </file>
@@ -22997,7 +23009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23051,13 +23063,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23585,12 +23598,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -71716,7 +71729,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -71748,7 +71761,7 @@
       <c r="F1" s="39" t="s">
         <v>7467</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="47" t="s">
         <v>7516</v>
       </c>
     </row>
@@ -71771,7 +71784,7 @@
       <c r="F2" s="40" t="s">
         <v>7473</v>
       </c>
-      <c r="G2" s="51" t="b">
+      <c r="G2" s="48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -71794,7 +71807,7 @@
       <c r="F3" s="40" t="s">
         <v>7478</v>
       </c>
-      <c r="G3" s="51" t="b">
+      <c r="G3" s="48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -71817,7 +71830,7 @@
       <c r="F4" s="40" t="s">
         <v>7483</v>
       </c>
-      <c r="G4" s="51" t="b">
+      <c r="G4" s="48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -71840,7 +71853,7 @@
       <c r="F5" s="40" t="s">
         <v>7489</v>
       </c>
-      <c r="G5" s="51" t="b">
+      <c r="G5" s="48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -71863,7 +71876,7 @@
       <c r="F6" s="40" t="s">
         <v>7494</v>
       </c>
-      <c r="G6" s="51" t="b">
+      <c r="G6" s="48" t="b">
         <v>1</v>
       </c>
     </row>
@@ -71886,17 +71899,30 @@
       <c r="F7" s="40" t="s">
         <v>7499</v>
       </c>
-      <c r="G7" s="51" t="b">
+      <c r="G7" s="48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="37"/>
-      <c r="G8" s="51"/>
+    <row r="8" spans="1:7" s="22" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="15" t="s">
+        <v>7517</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>7517</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="46" t="s">
+        <v>7518</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>7519</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>7520</v>
+      </c>
+      <c r="G8" s="48" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
@@ -71904,7 +71930,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="G9" s="51"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
@@ -71912,7 +71938,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="G10" s="51"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
@@ -71920,7 +71946,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="51"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -71928,7 +71954,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="51"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
@@ -71936,7 +71962,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="G13" s="51"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
@@ -71944,2965 +71970,2965 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="G14" s="51"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="G15" s="51"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="G16" s="51"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G17" s="51"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G18" s="51"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G19" s="51"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G20" s="51"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G21" s="51"/>
+      <c r="G21" s="48"/>
     </row>
     <row r="22" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G22" s="51"/>
+      <c r="G22" s="48"/>
     </row>
     <row r="23" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G23" s="51"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G24" s="51"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G25" s="51"/>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G26" s="51"/>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G27" s="51"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G28" s="51"/>
+      <c r="G28" s="48"/>
     </row>
     <row r="29" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G29" s="51"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G30" s="51"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G31" s="51"/>
+      <c r="G31" s="48"/>
     </row>
     <row r="32" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G32" s="51"/>
+      <c r="G32" s="48"/>
     </row>
     <row r="33" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G33" s="51"/>
+      <c r="G33" s="48"/>
     </row>
     <row r="34" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G34" s="51"/>
+      <c r="G34" s="48"/>
     </row>
     <row r="35" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G35" s="51"/>
+      <c r="G35" s="48"/>
     </row>
     <row r="36" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G36" s="51"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G37" s="51"/>
+      <c r="G37" s="48"/>
     </row>
     <row r="38" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G38" s="51"/>
+      <c r="G38" s="48"/>
     </row>
     <row r="39" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G39" s="51"/>
+      <c r="G39" s="48"/>
     </row>
     <row r="40" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G40" s="51"/>
+      <c r="G40" s="48"/>
     </row>
     <row r="41" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G41" s="51"/>
+      <c r="G41" s="48"/>
     </row>
     <row r="42" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G42" s="51"/>
+      <c r="G42" s="48"/>
     </row>
     <row r="43" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G43" s="51"/>
+      <c r="G43" s="48"/>
     </row>
     <row r="44" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G44" s="51"/>
+      <c r="G44" s="48"/>
     </row>
     <row r="45" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G45" s="51"/>
+      <c r="G45" s="48"/>
     </row>
     <row r="46" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G46" s="51"/>
+      <c r="G46" s="48"/>
     </row>
     <row r="47" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G47" s="51"/>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G48" s="51"/>
+      <c r="G48" s="48"/>
     </row>
     <row r="49" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G49" s="51"/>
+      <c r="G49" s="48"/>
     </row>
     <row r="50" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G50" s="51"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G51" s="51"/>
+      <c r="G51" s="48"/>
     </row>
     <row r="52" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G52" s="51"/>
+      <c r="G52" s="48"/>
     </row>
     <row r="53" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G53" s="51"/>
+      <c r="G53" s="48"/>
     </row>
     <row r="54" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G54" s="51"/>
+      <c r="G54" s="48"/>
     </row>
     <row r="55" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G55" s="51"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G56" s="51"/>
+      <c r="G56" s="48"/>
     </row>
     <row r="57" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G57" s="51"/>
+      <c r="G57" s="48"/>
     </row>
     <row r="58" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G58" s="51"/>
+      <c r="G58" s="48"/>
     </row>
     <row r="59" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G59" s="51"/>
+      <c r="G59" s="48"/>
     </row>
     <row r="60" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G60" s="51"/>
+      <c r="G60" s="48"/>
     </row>
     <row r="61" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G61" s="51"/>
+      <c r="G61" s="48"/>
     </row>
     <row r="62" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G62" s="51"/>
+      <c r="G62" s="48"/>
     </row>
     <row r="63" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G63" s="51"/>
+      <c r="G63" s="48"/>
     </row>
     <row r="64" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G64" s="51"/>
+      <c r="G64" s="48"/>
     </row>
     <row r="65" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G65" s="51"/>
+      <c r="G65" s="48"/>
     </row>
     <row r="66" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G66" s="51"/>
+      <c r="G66" s="48"/>
     </row>
     <row r="67" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G67" s="51"/>
+      <c r="G67" s="48"/>
     </row>
     <row r="68" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G68" s="51"/>
+      <c r="G68" s="48"/>
     </row>
     <row r="69" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G69" s="51"/>
+      <c r="G69" s="48"/>
     </row>
     <row r="70" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G70" s="51"/>
+      <c r="G70" s="48"/>
     </row>
     <row r="71" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G71" s="51"/>
+      <c r="G71" s="48"/>
     </row>
     <row r="72" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G72" s="51"/>
+      <c r="G72" s="48"/>
     </row>
     <row r="73" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G73" s="51"/>
+      <c r="G73" s="48"/>
     </row>
     <row r="74" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G74" s="51"/>
+      <c r="G74" s="48"/>
     </row>
     <row r="75" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G75" s="51"/>
+      <c r="G75" s="48"/>
     </row>
     <row r="76" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G76" s="51"/>
+      <c r="G76" s="48"/>
     </row>
     <row r="77" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G77" s="51"/>
+      <c r="G77" s="48"/>
     </row>
     <row r="78" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G78" s="51"/>
+      <c r="G78" s="48"/>
     </row>
     <row r="79" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G79" s="51"/>
+      <c r="G79" s="48"/>
     </row>
     <row r="80" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G80" s="51"/>
+      <c r="G80" s="48"/>
     </row>
     <row r="81" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G81" s="51"/>
+      <c r="G81" s="48"/>
     </row>
     <row r="82" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G82" s="51"/>
+      <c r="G82" s="48"/>
     </row>
     <row r="83" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G83" s="51"/>
+      <c r="G83" s="48"/>
     </row>
     <row r="84" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G84" s="51"/>
+      <c r="G84" s="48"/>
     </row>
     <row r="85" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G85" s="51"/>
+      <c r="G85" s="48"/>
     </row>
     <row r="86" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G86" s="51"/>
+      <c r="G86" s="48"/>
     </row>
     <row r="87" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G87" s="51"/>
+      <c r="G87" s="48"/>
     </row>
     <row r="88" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G88" s="51"/>
+      <c r="G88" s="48"/>
     </row>
     <row r="89" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G89" s="51"/>
+      <c r="G89" s="48"/>
     </row>
     <row r="90" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G90" s="51"/>
+      <c r="G90" s="48"/>
     </row>
     <row r="91" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G91" s="51"/>
+      <c r="G91" s="48"/>
     </row>
     <row r="92" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G92" s="51"/>
+      <c r="G92" s="48"/>
     </row>
     <row r="93" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G93" s="51"/>
+      <c r="G93" s="48"/>
     </row>
     <row r="94" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G94" s="51"/>
+      <c r="G94" s="48"/>
     </row>
     <row r="95" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G95" s="51"/>
+      <c r="G95" s="48"/>
     </row>
     <row r="96" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G96" s="51"/>
+      <c r="G96" s="48"/>
     </row>
     <row r="97" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G97" s="51"/>
+      <c r="G97" s="48"/>
     </row>
     <row r="98" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G98" s="51"/>
+      <c r="G98" s="48"/>
     </row>
     <row r="99" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G99" s="51"/>
+      <c r="G99" s="48"/>
     </row>
     <row r="100" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G100" s="51"/>
+      <c r="G100" s="48"/>
     </row>
     <row r="101" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G101" s="51"/>
+      <c r="G101" s="48"/>
     </row>
     <row r="102" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G102" s="51"/>
+      <c r="G102" s="48"/>
     </row>
     <row r="103" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G103" s="51"/>
+      <c r="G103" s="48"/>
     </row>
     <row r="104" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G104" s="51"/>
+      <c r="G104" s="48"/>
     </row>
     <row r="105" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G105" s="51"/>
+      <c r="G105" s="48"/>
     </row>
     <row r="106" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G106" s="51"/>
+      <c r="G106" s="48"/>
     </row>
     <row r="107" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G107" s="51"/>
+      <c r="G107" s="48"/>
     </row>
     <row r="108" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G108" s="51"/>
+      <c r="G108" s="48"/>
     </row>
     <row r="109" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G109" s="51"/>
+      <c r="G109" s="48"/>
     </row>
     <row r="110" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G110" s="51"/>
+      <c r="G110" s="48"/>
     </row>
     <row r="111" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G111" s="51"/>
+      <c r="G111" s="48"/>
     </row>
     <row r="112" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G112" s="51"/>
+      <c r="G112" s="48"/>
     </row>
     <row r="113" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G113" s="51"/>
+      <c r="G113" s="48"/>
     </row>
     <row r="114" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G114" s="51"/>
+      <c r="G114" s="48"/>
     </row>
     <row r="115" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G115" s="51"/>
+      <c r="G115" s="48"/>
     </row>
     <row r="116" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G116" s="51"/>
+      <c r="G116" s="48"/>
     </row>
     <row r="117" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G117" s="51"/>
+      <c r="G117" s="48"/>
     </row>
     <row r="118" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G118" s="51"/>
+      <c r="G118" s="48"/>
     </row>
     <row r="119" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G119" s="51"/>
+      <c r="G119" s="48"/>
     </row>
     <row r="120" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G120" s="51"/>
+      <c r="G120" s="48"/>
     </row>
     <row r="121" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G121" s="51"/>
+      <c r="G121" s="48"/>
     </row>
     <row r="122" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G122" s="51"/>
+      <c r="G122" s="48"/>
     </row>
     <row r="123" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G123" s="51"/>
+      <c r="G123" s="48"/>
     </row>
     <row r="124" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G124" s="51"/>
+      <c r="G124" s="48"/>
     </row>
     <row r="125" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G125" s="51"/>
+      <c r="G125" s="48"/>
     </row>
     <row r="126" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G126" s="51"/>
+      <c r="G126" s="48"/>
     </row>
     <row r="127" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G127" s="51"/>
+      <c r="G127" s="48"/>
     </row>
     <row r="128" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G128" s="51"/>
+      <c r="G128" s="48"/>
     </row>
     <row r="129" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G129" s="51"/>
+      <c r="G129" s="48"/>
     </row>
     <row r="130" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G130" s="51"/>
+      <c r="G130" s="48"/>
     </row>
     <row r="131" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G131" s="51"/>
+      <c r="G131" s="48"/>
     </row>
     <row r="132" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G132" s="51"/>
+      <c r="G132" s="48"/>
     </row>
     <row r="133" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G133" s="51"/>
+      <c r="G133" s="48"/>
     </row>
     <row r="134" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G134" s="51"/>
+      <c r="G134" s="48"/>
     </row>
     <row r="135" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G135" s="51"/>
+      <c r="G135" s="48"/>
     </row>
     <row r="136" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G136" s="51"/>
+      <c r="G136" s="48"/>
     </row>
     <row r="137" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G137" s="51"/>
+      <c r="G137" s="48"/>
     </row>
     <row r="138" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G138" s="51"/>
+      <c r="G138" s="48"/>
     </row>
     <row r="139" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G139" s="51"/>
+      <c r="G139" s="48"/>
     </row>
     <row r="140" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G140" s="51"/>
+      <c r="G140" s="48"/>
     </row>
     <row r="141" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G141" s="51"/>
+      <c r="G141" s="48"/>
     </row>
     <row r="142" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G142" s="51"/>
+      <c r="G142" s="48"/>
     </row>
     <row r="143" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G143" s="51"/>
+      <c r="G143" s="48"/>
     </row>
     <row r="144" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G144" s="51"/>
+      <c r="G144" s="48"/>
     </row>
     <row r="145" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G145" s="51"/>
+      <c r="G145" s="48"/>
     </row>
     <row r="146" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G146" s="51"/>
+      <c r="G146" s="48"/>
     </row>
     <row r="147" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G147" s="51"/>
+      <c r="G147" s="48"/>
     </row>
     <row r="148" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G148" s="51"/>
+      <c r="G148" s="48"/>
     </row>
     <row r="149" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G149" s="51"/>
+      <c r="G149" s="48"/>
     </row>
     <row r="150" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G150" s="51"/>
+      <c r="G150" s="48"/>
     </row>
     <row r="151" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G151" s="51"/>
+      <c r="G151" s="48"/>
     </row>
     <row r="152" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G152" s="51"/>
+      <c r="G152" s="48"/>
     </row>
     <row r="153" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G153" s="51"/>
+      <c r="G153" s="48"/>
     </row>
     <row r="154" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G154" s="51"/>
+      <c r="G154" s="48"/>
     </row>
     <row r="155" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G155" s="51"/>
+      <c r="G155" s="48"/>
     </row>
     <row r="156" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G156" s="51"/>
+      <c r="G156" s="48"/>
     </row>
     <row r="157" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G157" s="51"/>
+      <c r="G157" s="48"/>
     </row>
     <row r="158" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G158" s="51"/>
+      <c r="G158" s="48"/>
     </row>
     <row r="159" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G159" s="51"/>
+      <c r="G159" s="48"/>
     </row>
     <row r="160" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G160" s="51"/>
+      <c r="G160" s="48"/>
     </row>
     <row r="161" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G161" s="51"/>
+      <c r="G161" s="48"/>
     </row>
     <row r="162" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G162" s="51"/>
+      <c r="G162" s="48"/>
     </row>
     <row r="163" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G163" s="51"/>
+      <c r="G163" s="48"/>
     </row>
     <row r="164" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G164" s="51"/>
+      <c r="G164" s="48"/>
     </row>
     <row r="165" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G165" s="51"/>
+      <c r="G165" s="48"/>
     </row>
     <row r="166" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G166" s="51"/>
+      <c r="G166" s="48"/>
     </row>
     <row r="167" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G167" s="51"/>
+      <c r="G167" s="48"/>
     </row>
     <row r="168" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G168" s="51"/>
+      <c r="G168" s="48"/>
     </row>
     <row r="169" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G169" s="51"/>
+      <c r="G169" s="48"/>
     </row>
     <row r="170" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G170" s="51"/>
+      <c r="G170" s="48"/>
     </row>
     <row r="171" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G171" s="51"/>
+      <c r="G171" s="48"/>
     </row>
     <row r="172" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G172" s="51"/>
+      <c r="G172" s="48"/>
     </row>
     <row r="173" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G173" s="51"/>
+      <c r="G173" s="48"/>
     </row>
     <row r="174" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G174" s="51"/>
+      <c r="G174" s="48"/>
     </row>
     <row r="175" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G175" s="51"/>
+      <c r="G175" s="48"/>
     </row>
     <row r="176" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G176" s="51"/>
+      <c r="G176" s="48"/>
     </row>
     <row r="177" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G177" s="51"/>
+      <c r="G177" s="48"/>
     </row>
     <row r="178" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G178" s="51"/>
+      <c r="G178" s="48"/>
     </row>
     <row r="179" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G179" s="51"/>
+      <c r="G179" s="48"/>
     </row>
     <row r="180" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G180" s="51"/>
+      <c r="G180" s="48"/>
     </row>
     <row r="181" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G181" s="51"/>
+      <c r="G181" s="48"/>
     </row>
     <row r="182" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G182" s="51"/>
+      <c r="G182" s="48"/>
     </row>
     <row r="183" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G183" s="51"/>
+      <c r="G183" s="48"/>
     </row>
     <row r="184" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G184" s="51"/>
+      <c r="G184" s="48"/>
     </row>
     <row r="185" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G185" s="51"/>
+      <c r="G185" s="48"/>
     </row>
     <row r="186" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G186" s="51"/>
+      <c r="G186" s="48"/>
     </row>
     <row r="187" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G187" s="51"/>
+      <c r="G187" s="48"/>
     </row>
     <row r="188" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G188" s="51"/>
+      <c r="G188" s="48"/>
     </row>
     <row r="189" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G189" s="51"/>
+      <c r="G189" s="48"/>
     </row>
     <row r="190" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G190" s="51"/>
+      <c r="G190" s="48"/>
     </row>
     <row r="191" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G191" s="51"/>
+      <c r="G191" s="48"/>
     </row>
     <row r="192" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G192" s="51"/>
+      <c r="G192" s="48"/>
     </row>
     <row r="193" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G193" s="51"/>
+      <c r="G193" s="48"/>
     </row>
     <row r="194" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G194" s="51"/>
+      <c r="G194" s="48"/>
     </row>
     <row r="195" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G195" s="51"/>
+      <c r="G195" s="48"/>
     </row>
     <row r="196" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G196" s="51"/>
+      <c r="G196" s="48"/>
     </row>
     <row r="197" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G197" s="51"/>
+      <c r="G197" s="48"/>
     </row>
     <row r="198" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G198" s="51"/>
+      <c r="G198" s="48"/>
     </row>
     <row r="199" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G199" s="51"/>
+      <c r="G199" s="48"/>
     </row>
     <row r="200" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G200" s="51"/>
+      <c r="G200" s="48"/>
     </row>
     <row r="201" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G201" s="51"/>
+      <c r="G201" s="48"/>
     </row>
     <row r="202" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G202" s="51"/>
+      <c r="G202" s="48"/>
     </row>
     <row r="203" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G203" s="51"/>
+      <c r="G203" s="48"/>
     </row>
     <row r="204" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G204" s="51"/>
+      <c r="G204" s="48"/>
     </row>
     <row r="205" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G205" s="51"/>
+      <c r="G205" s="48"/>
     </row>
     <row r="206" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G206" s="51"/>
+      <c r="G206" s="48"/>
     </row>
     <row r="207" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G207" s="51"/>
+      <c r="G207" s="48"/>
     </row>
     <row r="208" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G208" s="51"/>
+      <c r="G208" s="48"/>
     </row>
     <row r="209" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G209" s="51"/>
+      <c r="G209" s="48"/>
     </row>
     <row r="210" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G210" s="51"/>
+      <c r="G210" s="48"/>
     </row>
     <row r="211" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G211" s="51"/>
+      <c r="G211" s="48"/>
     </row>
     <row r="212" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G212" s="51"/>
+      <c r="G212" s="48"/>
     </row>
     <row r="213" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G213" s="51"/>
+      <c r="G213" s="48"/>
     </row>
     <row r="214" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G214" s="51"/>
+      <c r="G214" s="48"/>
     </row>
     <row r="215" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G215" s="51"/>
+      <c r="G215" s="48"/>
     </row>
     <row r="216" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G216" s="51"/>
+      <c r="G216" s="48"/>
     </row>
     <row r="217" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G217" s="51"/>
+      <c r="G217" s="48"/>
     </row>
     <row r="218" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G218" s="51"/>
+      <c r="G218" s="48"/>
     </row>
     <row r="219" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G219" s="51"/>
+      <c r="G219" s="48"/>
     </row>
     <row r="220" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G220" s="51"/>
+      <c r="G220" s="48"/>
     </row>
     <row r="221" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G221" s="51"/>
+      <c r="G221" s="48"/>
     </row>
     <row r="222" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G222" s="51"/>
+      <c r="G222" s="48"/>
     </row>
     <row r="223" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G223" s="51"/>
+      <c r="G223" s="48"/>
     </row>
     <row r="224" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G224" s="51"/>
+      <c r="G224" s="48"/>
     </row>
     <row r="225" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G225" s="51"/>
+      <c r="G225" s="48"/>
     </row>
     <row r="226" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G226" s="51"/>
+      <c r="G226" s="48"/>
     </row>
     <row r="227" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G227" s="51"/>
+      <c r="G227" s="48"/>
     </row>
     <row r="228" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G228" s="51"/>
+      <c r="G228" s="48"/>
     </row>
     <row r="229" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G229" s="51"/>
+      <c r="G229" s="48"/>
     </row>
     <row r="230" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G230" s="51"/>
+      <c r="G230" s="48"/>
     </row>
     <row r="231" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G231" s="51"/>
+      <c r="G231" s="48"/>
     </row>
     <row r="232" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G232" s="51"/>
+      <c r="G232" s="48"/>
     </row>
     <row r="233" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G233" s="51"/>
+      <c r="G233" s="48"/>
     </row>
     <row r="234" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G234" s="51"/>
+      <c r="G234" s="48"/>
     </row>
     <row r="235" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G235" s="51"/>
+      <c r="G235" s="48"/>
     </row>
     <row r="236" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G236" s="51"/>
+      <c r="G236" s="48"/>
     </row>
     <row r="237" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G237" s="51"/>
+      <c r="G237" s="48"/>
     </row>
     <row r="238" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G238" s="51"/>
+      <c r="G238" s="48"/>
     </row>
     <row r="239" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G239" s="51"/>
+      <c r="G239" s="48"/>
     </row>
     <row r="240" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G240" s="51"/>
+      <c r="G240" s="48"/>
     </row>
     <row r="241" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G241" s="51"/>
+      <c r="G241" s="48"/>
     </row>
     <row r="242" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G242" s="51"/>
+      <c r="G242" s="48"/>
     </row>
     <row r="243" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G243" s="51"/>
+      <c r="G243" s="48"/>
     </row>
     <row r="244" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G244" s="51"/>
+      <c r="G244" s="48"/>
     </row>
     <row r="245" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G245" s="51"/>
+      <c r="G245" s="48"/>
     </row>
     <row r="246" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G246" s="51"/>
+      <c r="G246" s="48"/>
     </row>
     <row r="247" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G247" s="51"/>
+      <c r="G247" s="48"/>
     </row>
     <row r="248" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G248" s="51"/>
+      <c r="G248" s="48"/>
     </row>
     <row r="249" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G249" s="51"/>
+      <c r="G249" s="48"/>
     </row>
     <row r="250" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G250" s="51"/>
+      <c r="G250" s="48"/>
     </row>
     <row r="251" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G251" s="51"/>
+      <c r="G251" s="48"/>
     </row>
     <row r="252" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G252" s="51"/>
+      <c r="G252" s="48"/>
     </row>
     <row r="253" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G253" s="51"/>
+      <c r="G253" s="48"/>
     </row>
     <row r="254" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G254" s="51"/>
+      <c r="G254" s="48"/>
     </row>
     <row r="255" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G255" s="51"/>
+      <c r="G255" s="48"/>
     </row>
     <row r="256" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G256" s="51"/>
+      <c r="G256" s="48"/>
     </row>
     <row r="257" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G257" s="51"/>
+      <c r="G257" s="48"/>
     </row>
     <row r="258" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G258" s="51"/>
+      <c r="G258" s="48"/>
     </row>
     <row r="259" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G259" s="51"/>
+      <c r="G259" s="48"/>
     </row>
     <row r="260" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G260" s="51"/>
+      <c r="G260" s="48"/>
     </row>
     <row r="261" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G261" s="51"/>
+      <c r="G261" s="48"/>
     </row>
     <row r="262" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G262" s="51"/>
+      <c r="G262" s="48"/>
     </row>
     <row r="263" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G263" s="51"/>
+      <c r="G263" s="48"/>
     </row>
     <row r="264" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G264" s="51"/>
+      <c r="G264" s="48"/>
     </row>
     <row r="265" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G265" s="51"/>
+      <c r="G265" s="48"/>
     </row>
     <row r="266" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G266" s="51"/>
+      <c r="G266" s="48"/>
     </row>
     <row r="267" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G267" s="51"/>
+      <c r="G267" s="48"/>
     </row>
     <row r="268" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G268" s="51"/>
+      <c r="G268" s="48"/>
     </row>
     <row r="269" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G269" s="51"/>
+      <c r="G269" s="48"/>
     </row>
     <row r="270" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G270" s="51"/>
+      <c r="G270" s="48"/>
     </row>
     <row r="271" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G271" s="51"/>
+      <c r="G271" s="48"/>
     </row>
     <row r="272" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G272" s="51"/>
+      <c r="G272" s="48"/>
     </row>
     <row r="273" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G273" s="51"/>
+      <c r="G273" s="48"/>
     </row>
     <row r="274" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G274" s="51"/>
+      <c r="G274" s="48"/>
     </row>
     <row r="275" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G275" s="51"/>
+      <c r="G275" s="48"/>
     </row>
     <row r="276" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G276" s="51"/>
+      <c r="G276" s="48"/>
     </row>
     <row r="277" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G277" s="51"/>
+      <c r="G277" s="48"/>
     </row>
     <row r="278" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G278" s="51"/>
+      <c r="G278" s="48"/>
     </row>
     <row r="279" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G279" s="51"/>
+      <c r="G279" s="48"/>
     </row>
     <row r="280" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G280" s="51"/>
+      <c r="G280" s="48"/>
     </row>
     <row r="281" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G281" s="51"/>
+      <c r="G281" s="48"/>
     </row>
     <row r="282" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G282" s="51"/>
+      <c r="G282" s="48"/>
     </row>
     <row r="283" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G283" s="51"/>
+      <c r="G283" s="48"/>
     </row>
     <row r="284" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G284" s="51"/>
+      <c r="G284" s="48"/>
     </row>
     <row r="285" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G285" s="51"/>
+      <c r="G285" s="48"/>
     </row>
     <row r="286" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G286" s="51"/>
+      <c r="G286" s="48"/>
     </row>
     <row r="287" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G287" s="51"/>
+      <c r="G287" s="48"/>
     </row>
     <row r="288" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G288" s="51"/>
+      <c r="G288" s="48"/>
     </row>
     <row r="289" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G289" s="51"/>
+      <c r="G289" s="48"/>
     </row>
     <row r="290" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G290" s="51"/>
+      <c r="G290" s="48"/>
     </row>
     <row r="291" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G291" s="51"/>
+      <c r="G291" s="48"/>
     </row>
     <row r="292" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G292" s="51"/>
+      <c r="G292" s="48"/>
     </row>
     <row r="293" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G293" s="51"/>
+      <c r="G293" s="48"/>
     </row>
     <row r="294" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G294" s="51"/>
+      <c r="G294" s="48"/>
     </row>
     <row r="295" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G295" s="51"/>
+      <c r="G295" s="48"/>
     </row>
     <row r="296" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G296" s="51"/>
+      <c r="G296" s="48"/>
     </row>
     <row r="297" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G297" s="51"/>
+      <c r="G297" s="48"/>
     </row>
     <row r="298" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G298" s="51"/>
+      <c r="G298" s="48"/>
     </row>
     <row r="299" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G299" s="51"/>
+      <c r="G299" s="48"/>
     </row>
     <row r="300" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G300" s="51"/>
+      <c r="G300" s="48"/>
     </row>
     <row r="301" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G301" s="51"/>
+      <c r="G301" s="48"/>
     </row>
     <row r="302" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G302" s="51"/>
+      <c r="G302" s="48"/>
     </row>
     <row r="303" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G303" s="51"/>
+      <c r="G303" s="48"/>
     </row>
     <row r="304" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G304" s="51"/>
+      <c r="G304" s="48"/>
     </row>
     <row r="305" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G305" s="51"/>
+      <c r="G305" s="48"/>
     </row>
     <row r="306" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G306" s="51"/>
+      <c r="G306" s="48"/>
     </row>
     <row r="307" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G307" s="51"/>
+      <c r="G307" s="48"/>
     </row>
     <row r="308" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G308" s="51"/>
+      <c r="G308" s="48"/>
     </row>
     <row r="309" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G309" s="51"/>
+      <c r="G309" s="48"/>
     </row>
     <row r="310" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G310" s="51"/>
+      <c r="G310" s="48"/>
     </row>
     <row r="311" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G311" s="51"/>
+      <c r="G311" s="48"/>
     </row>
     <row r="312" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G312" s="51"/>
+      <c r="G312" s="48"/>
     </row>
     <row r="313" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G313" s="51"/>
+      <c r="G313" s="48"/>
     </row>
     <row r="314" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G314" s="51"/>
+      <c r="G314" s="48"/>
     </row>
     <row r="315" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G315" s="51"/>
+      <c r="G315" s="48"/>
     </row>
     <row r="316" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G316" s="51"/>
+      <c r="G316" s="48"/>
     </row>
     <row r="317" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G317" s="51"/>
+      <c r="G317" s="48"/>
     </row>
     <row r="318" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G318" s="51"/>
+      <c r="G318" s="48"/>
     </row>
     <row r="319" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G319" s="51"/>
+      <c r="G319" s="48"/>
     </row>
     <row r="320" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G320" s="51"/>
+      <c r="G320" s="48"/>
     </row>
     <row r="321" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G321" s="51"/>
+      <c r="G321" s="48"/>
     </row>
     <row r="322" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G322" s="51"/>
+      <c r="G322" s="48"/>
     </row>
     <row r="323" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G323" s="51"/>
+      <c r="G323" s="48"/>
     </row>
     <row r="324" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G324" s="51"/>
+      <c r="G324" s="48"/>
     </row>
     <row r="325" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G325" s="51"/>
+      <c r="G325" s="48"/>
     </row>
     <row r="326" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G326" s="51"/>
+      <c r="G326" s="48"/>
     </row>
     <row r="327" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G327" s="51"/>
+      <c r="G327" s="48"/>
     </row>
     <row r="328" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G328" s="51"/>
+      <c r="G328" s="48"/>
     </row>
     <row r="329" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G329" s="51"/>
+      <c r="G329" s="48"/>
     </row>
     <row r="330" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G330" s="51"/>
+      <c r="G330" s="48"/>
     </row>
     <row r="331" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G331" s="51"/>
+      <c r="G331" s="48"/>
     </row>
     <row r="332" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G332" s="51"/>
+      <c r="G332" s="48"/>
     </row>
     <row r="333" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G333" s="51"/>
+      <c r="G333" s="48"/>
     </row>
     <row r="334" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G334" s="51"/>
+      <c r="G334" s="48"/>
     </row>
     <row r="335" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G335" s="51"/>
+      <c r="G335" s="48"/>
     </row>
     <row r="336" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G336" s="51"/>
+      <c r="G336" s="48"/>
     </row>
     <row r="337" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G337" s="51"/>
+      <c r="G337" s="48"/>
     </row>
     <row r="338" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G338" s="51"/>
+      <c r="G338" s="48"/>
     </row>
     <row r="339" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G339" s="51"/>
+      <c r="G339" s="48"/>
     </row>
     <row r="340" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G340" s="51"/>
+      <c r="G340" s="48"/>
     </row>
     <row r="341" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G341" s="51"/>
+      <c r="G341" s="48"/>
     </row>
     <row r="342" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G342" s="51"/>
+      <c r="G342" s="48"/>
     </row>
     <row r="343" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G343" s="51"/>
+      <c r="G343" s="48"/>
     </row>
     <row r="344" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G344" s="51"/>
+      <c r="G344" s="48"/>
     </row>
     <row r="345" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G345" s="51"/>
+      <c r="G345" s="48"/>
     </row>
     <row r="346" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G346" s="51"/>
+      <c r="G346" s="48"/>
     </row>
     <row r="347" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G347" s="51"/>
+      <c r="G347" s="48"/>
     </row>
     <row r="348" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G348" s="51"/>
+      <c r="G348" s="48"/>
     </row>
     <row r="349" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G349" s="51"/>
+      <c r="G349" s="48"/>
     </row>
     <row r="350" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G350" s="51"/>
+      <c r="G350" s="48"/>
     </row>
     <row r="351" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G351" s="51"/>
+      <c r="G351" s="48"/>
     </row>
     <row r="352" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G352" s="51"/>
+      <c r="G352" s="48"/>
     </row>
     <row r="353" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G353" s="51"/>
+      <c r="G353" s="48"/>
     </row>
     <row r="354" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G354" s="51"/>
+      <c r="G354" s="48"/>
     </row>
     <row r="355" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G355" s="51"/>
+      <c r="G355" s="48"/>
     </row>
     <row r="356" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G356" s="51"/>
+      <c r="G356" s="48"/>
     </row>
     <row r="357" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G357" s="51"/>
+      <c r="G357" s="48"/>
     </row>
     <row r="358" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G358" s="51"/>
+      <c r="G358" s="48"/>
     </row>
     <row r="359" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G359" s="51"/>
+      <c r="G359" s="48"/>
     </row>
     <row r="360" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G360" s="51"/>
+      <c r="G360" s="48"/>
     </row>
     <row r="361" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G361" s="51"/>
+      <c r="G361" s="48"/>
     </row>
     <row r="362" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G362" s="51"/>
+      <c r="G362" s="48"/>
     </row>
     <row r="363" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G363" s="51"/>
+      <c r="G363" s="48"/>
     </row>
     <row r="364" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G364" s="51"/>
+      <c r="G364" s="48"/>
     </row>
     <row r="365" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G365" s="51"/>
+      <c r="G365" s="48"/>
     </row>
     <row r="366" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G366" s="51"/>
+      <c r="G366" s="48"/>
     </row>
     <row r="367" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G367" s="51"/>
+      <c r="G367" s="48"/>
     </row>
     <row r="368" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G368" s="51"/>
+      <c r="G368" s="48"/>
     </row>
     <row r="369" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G369" s="51"/>
+      <c r="G369" s="48"/>
     </row>
     <row r="370" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G370" s="51"/>
+      <c r="G370" s="48"/>
     </row>
     <row r="371" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G371" s="51"/>
+      <c r="G371" s="48"/>
     </row>
     <row r="372" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G372" s="51"/>
+      <c r="G372" s="48"/>
     </row>
     <row r="373" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G373" s="51"/>
+      <c r="G373" s="48"/>
     </row>
     <row r="374" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G374" s="51"/>
+      <c r="G374" s="48"/>
     </row>
     <row r="375" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G375" s="51"/>
+      <c r="G375" s="48"/>
     </row>
     <row r="376" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G376" s="51"/>
+      <c r="G376" s="48"/>
     </row>
     <row r="377" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G377" s="51"/>
+      <c r="G377" s="48"/>
     </row>
     <row r="378" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G378" s="51"/>
+      <c r="G378" s="48"/>
     </row>
     <row r="379" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G379" s="51"/>
+      <c r="G379" s="48"/>
     </row>
     <row r="380" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G380" s="51"/>
+      <c r="G380" s="48"/>
     </row>
     <row r="381" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G381" s="51"/>
+      <c r="G381" s="48"/>
     </row>
     <row r="382" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G382" s="51"/>
+      <c r="G382" s="48"/>
     </row>
     <row r="383" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G383" s="51"/>
+      <c r="G383" s="48"/>
     </row>
     <row r="384" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G384" s="51"/>
+      <c r="G384" s="48"/>
     </row>
     <row r="385" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G385" s="51"/>
+      <c r="G385" s="48"/>
     </row>
     <row r="386" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G386" s="51"/>
+      <c r="G386" s="48"/>
     </row>
     <row r="387" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G387" s="51"/>
+      <c r="G387" s="48"/>
     </row>
     <row r="388" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G388" s="51"/>
+      <c r="G388" s="48"/>
     </row>
     <row r="389" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G389" s="51"/>
+      <c r="G389" s="48"/>
     </row>
     <row r="390" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G390" s="51"/>
+      <c r="G390" s="48"/>
     </row>
     <row r="391" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G391" s="51"/>
+      <c r="G391" s="48"/>
     </row>
     <row r="392" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G392" s="51"/>
+      <c r="G392" s="48"/>
     </row>
     <row r="393" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G393" s="51"/>
+      <c r="G393" s="48"/>
     </row>
     <row r="394" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G394" s="51"/>
+      <c r="G394" s="48"/>
     </row>
     <row r="395" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G395" s="51"/>
+      <c r="G395" s="48"/>
     </row>
     <row r="396" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G396" s="51"/>
+      <c r="G396" s="48"/>
     </row>
     <row r="397" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G397" s="51"/>
+      <c r="G397" s="48"/>
     </row>
     <row r="398" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G398" s="51"/>
+      <c r="G398" s="48"/>
     </row>
     <row r="399" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G399" s="51"/>
+      <c r="G399" s="48"/>
     </row>
     <row r="400" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G400" s="51"/>
+      <c r="G400" s="48"/>
     </row>
     <row r="401" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G401" s="51"/>
+      <c r="G401" s="48"/>
     </row>
     <row r="402" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G402" s="51"/>
+      <c r="G402" s="48"/>
     </row>
     <row r="403" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G403" s="51"/>
+      <c r="G403" s="48"/>
     </row>
     <row r="404" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G404" s="51"/>
+      <c r="G404" s="48"/>
     </row>
     <row r="405" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G405" s="51"/>
+      <c r="G405" s="48"/>
     </row>
     <row r="406" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G406" s="51"/>
+      <c r="G406" s="48"/>
     </row>
     <row r="407" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G407" s="51"/>
+      <c r="G407" s="48"/>
     </row>
     <row r="408" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G408" s="51"/>
+      <c r="G408" s="48"/>
     </row>
     <row r="409" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G409" s="51"/>
+      <c r="G409" s="48"/>
     </row>
     <row r="410" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G410" s="51"/>
+      <c r="G410" s="48"/>
     </row>
     <row r="411" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G411" s="51"/>
+      <c r="G411" s="48"/>
     </row>
     <row r="412" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G412" s="51"/>
+      <c r="G412" s="48"/>
     </row>
     <row r="413" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G413" s="51"/>
+      <c r="G413" s="48"/>
     </row>
     <row r="414" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G414" s="51"/>
+      <c r="G414" s="48"/>
     </row>
     <row r="415" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G415" s="51"/>
+      <c r="G415" s="48"/>
     </row>
     <row r="416" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G416" s="51"/>
+      <c r="G416" s="48"/>
     </row>
     <row r="417" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G417" s="51"/>
+      <c r="G417" s="48"/>
     </row>
     <row r="418" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G418" s="51"/>
+      <c r="G418" s="48"/>
     </row>
     <row r="419" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G419" s="51"/>
+      <c r="G419" s="48"/>
     </row>
     <row r="420" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G420" s="51"/>
+      <c r="G420" s="48"/>
     </row>
     <row r="421" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G421" s="51"/>
+      <c r="G421" s="48"/>
     </row>
     <row r="422" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G422" s="51"/>
+      <c r="G422" s="48"/>
     </row>
     <row r="423" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G423" s="51"/>
+      <c r="G423" s="48"/>
     </row>
     <row r="424" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G424" s="51"/>
+      <c r="G424" s="48"/>
     </row>
     <row r="425" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G425" s="51"/>
+      <c r="G425" s="48"/>
     </row>
     <row r="426" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G426" s="51"/>
+      <c r="G426" s="48"/>
     </row>
     <row r="427" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G427" s="51"/>
+      <c r="G427" s="48"/>
     </row>
     <row r="428" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G428" s="51"/>
+      <c r="G428" s="48"/>
     </row>
     <row r="429" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G429" s="51"/>
+      <c r="G429" s="48"/>
     </row>
     <row r="430" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G430" s="51"/>
+      <c r="G430" s="48"/>
     </row>
     <row r="431" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G431" s="51"/>
+      <c r="G431" s="48"/>
     </row>
     <row r="432" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G432" s="51"/>
+      <c r="G432" s="48"/>
     </row>
     <row r="433" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G433" s="51"/>
+      <c r="G433" s="48"/>
     </row>
     <row r="434" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G434" s="51"/>
+      <c r="G434" s="48"/>
     </row>
     <row r="435" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G435" s="51"/>
+      <c r="G435" s="48"/>
     </row>
     <row r="436" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G436" s="51"/>
+      <c r="G436" s="48"/>
     </row>
     <row r="437" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G437" s="51"/>
+      <c r="G437" s="48"/>
     </row>
     <row r="438" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G438" s="51"/>
+      <c r="G438" s="48"/>
     </row>
     <row r="439" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G439" s="51"/>
+      <c r="G439" s="48"/>
     </row>
     <row r="440" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G440" s="51"/>
+      <c r="G440" s="48"/>
     </row>
     <row r="441" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G441" s="51"/>
+      <c r="G441" s="48"/>
     </row>
     <row r="442" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G442" s="51"/>
+      <c r="G442" s="48"/>
     </row>
     <row r="443" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G443" s="51"/>
+      <c r="G443" s="48"/>
     </row>
     <row r="444" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G444" s="51"/>
+      <c r="G444" s="48"/>
     </row>
     <row r="445" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G445" s="51"/>
+      <c r="G445" s="48"/>
     </row>
     <row r="446" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G446" s="51"/>
+      <c r="G446" s="48"/>
     </row>
     <row r="447" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G447" s="51"/>
+      <c r="G447" s="48"/>
     </row>
     <row r="448" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G448" s="51"/>
+      <c r="G448" s="48"/>
     </row>
     <row r="449" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G449" s="51"/>
+      <c r="G449" s="48"/>
     </row>
     <row r="450" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G450" s="51"/>
+      <c r="G450" s="48"/>
     </row>
     <row r="451" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G451" s="51"/>
+      <c r="G451" s="48"/>
     </row>
     <row r="452" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G452" s="51"/>
+      <c r="G452" s="48"/>
     </row>
     <row r="453" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G453" s="51"/>
+      <c r="G453" s="48"/>
     </row>
     <row r="454" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G454" s="51"/>
+      <c r="G454" s="48"/>
     </row>
     <row r="455" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G455" s="51"/>
+      <c r="G455" s="48"/>
     </row>
     <row r="456" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G456" s="51"/>
+      <c r="G456" s="48"/>
     </row>
     <row r="457" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G457" s="51"/>
+      <c r="G457" s="48"/>
     </row>
     <row r="458" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G458" s="51"/>
+      <c r="G458" s="48"/>
     </row>
     <row r="459" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G459" s="51"/>
+      <c r="G459" s="48"/>
     </row>
     <row r="460" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G460" s="51"/>
+      <c r="G460" s="48"/>
     </row>
     <row r="461" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G461" s="51"/>
+      <c r="G461" s="48"/>
     </row>
     <row r="462" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G462" s="51"/>
+      <c r="G462" s="48"/>
     </row>
     <row r="463" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G463" s="51"/>
+      <c r="G463" s="48"/>
     </row>
     <row r="464" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G464" s="51"/>
+      <c r="G464" s="48"/>
     </row>
     <row r="465" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G465" s="51"/>
+      <c r="G465" s="48"/>
     </row>
     <row r="466" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G466" s="51"/>
+      <c r="G466" s="48"/>
     </row>
     <row r="467" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G467" s="51"/>
+      <c r="G467" s="48"/>
     </row>
     <row r="468" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G468" s="51"/>
+      <c r="G468" s="48"/>
     </row>
     <row r="469" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G469" s="51"/>
+      <c r="G469" s="48"/>
     </row>
     <row r="470" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G470" s="51"/>
+      <c r="G470" s="48"/>
     </row>
     <row r="471" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G471" s="51"/>
+      <c r="G471" s="48"/>
     </row>
     <row r="472" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G472" s="51"/>
+      <c r="G472" s="48"/>
     </row>
     <row r="473" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G473" s="51"/>
+      <c r="G473" s="48"/>
     </row>
     <row r="474" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G474" s="51"/>
+      <c r="G474" s="48"/>
     </row>
     <row r="475" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G475" s="51"/>
+      <c r="G475" s="48"/>
     </row>
     <row r="476" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G476" s="51"/>
+      <c r="G476" s="48"/>
     </row>
     <row r="477" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G477" s="51"/>
+      <c r="G477" s="48"/>
     </row>
     <row r="478" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G478" s="51"/>
+      <c r="G478" s="48"/>
     </row>
     <row r="479" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G479" s="51"/>
+      <c r="G479" s="48"/>
     </row>
     <row r="480" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G480" s="51"/>
+      <c r="G480" s="48"/>
     </row>
     <row r="481" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G481" s="51"/>
+      <c r="G481" s="48"/>
     </row>
     <row r="482" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G482" s="51"/>
+      <c r="G482" s="48"/>
     </row>
     <row r="483" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G483" s="51"/>
+      <c r="G483" s="48"/>
     </row>
     <row r="484" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G484" s="51"/>
+      <c r="G484" s="48"/>
     </row>
     <row r="485" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G485" s="51"/>
+      <c r="G485" s="48"/>
     </row>
     <row r="486" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G486" s="51"/>
+      <c r="G486" s="48"/>
     </row>
     <row r="487" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G487" s="51"/>
+      <c r="G487" s="48"/>
     </row>
     <row r="488" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G488" s="51"/>
+      <c r="G488" s="48"/>
     </row>
     <row r="489" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G489" s="51"/>
+      <c r="G489" s="48"/>
     </row>
     <row r="490" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G490" s="51"/>
+      <c r="G490" s="48"/>
     </row>
     <row r="491" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G491" s="51"/>
+      <c r="G491" s="48"/>
     </row>
     <row r="492" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G492" s="51"/>
+      <c r="G492" s="48"/>
     </row>
     <row r="493" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G493" s="51"/>
+      <c r="G493" s="48"/>
     </row>
     <row r="494" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G494" s="51"/>
+      <c r="G494" s="48"/>
     </row>
     <row r="495" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G495" s="51"/>
+      <c r="G495" s="48"/>
     </row>
     <row r="496" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G496" s="51"/>
+      <c r="G496" s="48"/>
     </row>
     <row r="497" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G497" s="51"/>
+      <c r="G497" s="48"/>
     </row>
     <row r="498" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G498" s="51"/>
+      <c r="G498" s="48"/>
     </row>
     <row r="499" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G499" s="51"/>
+      <c r="G499" s="48"/>
     </row>
     <row r="500" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G500" s="51"/>
+      <c r="G500" s="48"/>
     </row>
     <row r="501" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G501" s="51"/>
+      <c r="G501" s="48"/>
     </row>
     <row r="502" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G502" s="51"/>
+      <c r="G502" s="48"/>
     </row>
     <row r="503" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G503" s="51"/>
+      <c r="G503" s="48"/>
     </row>
     <row r="504" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G504" s="51"/>
+      <c r="G504" s="48"/>
     </row>
     <row r="505" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G505" s="51"/>
+      <c r="G505" s="48"/>
     </row>
     <row r="506" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G506" s="51"/>
+      <c r="G506" s="48"/>
     </row>
     <row r="507" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G507" s="51"/>
+      <c r="G507" s="48"/>
     </row>
     <row r="508" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G508" s="51"/>
+      <c r="G508" s="48"/>
     </row>
     <row r="509" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G509" s="51"/>
+      <c r="G509" s="48"/>
     </row>
     <row r="510" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G510" s="51"/>
+      <c r="G510" s="48"/>
     </row>
     <row r="511" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G511" s="51"/>
+      <c r="G511" s="48"/>
     </row>
     <row r="512" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G512" s="51"/>
+      <c r="G512" s="48"/>
     </row>
     <row r="513" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G513" s="51"/>
+      <c r="G513" s="48"/>
     </row>
     <row r="514" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G514" s="51"/>
+      <c r="G514" s="48"/>
     </row>
     <row r="515" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G515" s="51"/>
+      <c r="G515" s="48"/>
     </row>
     <row r="516" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G516" s="51"/>
+      <c r="G516" s="48"/>
     </row>
     <row r="517" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G517" s="51"/>
+      <c r="G517" s="48"/>
     </row>
     <row r="518" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G518" s="51"/>
+      <c r="G518" s="48"/>
     </row>
     <row r="519" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G519" s="51"/>
+      <c r="G519" s="48"/>
     </row>
     <row r="520" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G520" s="51"/>
+      <c r="G520" s="48"/>
     </row>
     <row r="521" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G521" s="51"/>
+      <c r="G521" s="48"/>
     </row>
     <row r="522" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G522" s="51"/>
+      <c r="G522" s="48"/>
     </row>
     <row r="523" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G523" s="51"/>
+      <c r="G523" s="48"/>
     </row>
     <row r="524" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G524" s="51"/>
+      <c r="G524" s="48"/>
     </row>
     <row r="525" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G525" s="51"/>
+      <c r="G525" s="48"/>
     </row>
     <row r="526" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G526" s="51"/>
+      <c r="G526" s="48"/>
     </row>
     <row r="527" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G527" s="51"/>
+      <c r="G527" s="48"/>
     </row>
     <row r="528" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G528" s="51"/>
+      <c r="G528" s="48"/>
     </row>
     <row r="529" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G529" s="51"/>
+      <c r="G529" s="48"/>
     </row>
     <row r="530" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G530" s="51"/>
+      <c r="G530" s="48"/>
     </row>
     <row r="531" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G531" s="51"/>
+      <c r="G531" s="48"/>
     </row>
     <row r="532" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G532" s="51"/>
+      <c r="G532" s="48"/>
     </row>
     <row r="533" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G533" s="51"/>
+      <c r="G533" s="48"/>
     </row>
     <row r="534" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G534" s="51"/>
+      <c r="G534" s="48"/>
     </row>
     <row r="535" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G535" s="51"/>
+      <c r="G535" s="48"/>
     </row>
     <row r="536" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G536" s="51"/>
+      <c r="G536" s="48"/>
     </row>
     <row r="537" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G537" s="51"/>
+      <c r="G537" s="48"/>
     </row>
     <row r="538" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G538" s="51"/>
+      <c r="G538" s="48"/>
     </row>
     <row r="539" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G539" s="51"/>
+      <c r="G539" s="48"/>
     </row>
     <row r="540" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G540" s="51"/>
+      <c r="G540" s="48"/>
     </row>
     <row r="541" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G541" s="51"/>
+      <c r="G541" s="48"/>
     </row>
     <row r="542" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G542" s="51"/>
+      <c r="G542" s="48"/>
     </row>
     <row r="543" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G543" s="51"/>
+      <c r="G543" s="48"/>
     </row>
     <row r="544" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G544" s="51"/>
+      <c r="G544" s="48"/>
     </row>
     <row r="545" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G545" s="51"/>
+      <c r="G545" s="48"/>
     </row>
     <row r="546" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G546" s="51"/>
+      <c r="G546" s="48"/>
     </row>
     <row r="547" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G547" s="51"/>
+      <c r="G547" s="48"/>
     </row>
     <row r="548" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G548" s="51"/>
+      <c r="G548" s="48"/>
     </row>
     <row r="549" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G549" s="51"/>
+      <c r="G549" s="48"/>
     </row>
     <row r="550" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G550" s="51"/>
+      <c r="G550" s="48"/>
     </row>
     <row r="551" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G551" s="51"/>
+      <c r="G551" s="48"/>
     </row>
     <row r="552" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G552" s="51"/>
+      <c r="G552" s="48"/>
     </row>
     <row r="553" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G553" s="51"/>
+      <c r="G553" s="48"/>
     </row>
     <row r="554" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G554" s="51"/>
+      <c r="G554" s="48"/>
     </row>
     <row r="555" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G555" s="51"/>
+      <c r="G555" s="48"/>
     </row>
     <row r="556" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G556" s="51"/>
+      <c r="G556" s="48"/>
     </row>
     <row r="557" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G557" s="51"/>
+      <c r="G557" s="48"/>
     </row>
     <row r="558" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G558" s="51"/>
+      <c r="G558" s="48"/>
     </row>
     <row r="559" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G559" s="51"/>
+      <c r="G559" s="48"/>
     </row>
     <row r="560" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G560" s="51"/>
+      <c r="G560" s="48"/>
     </row>
     <row r="561" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G561" s="51"/>
+      <c r="G561" s="48"/>
     </row>
     <row r="562" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G562" s="51"/>
+      <c r="G562" s="48"/>
     </row>
     <row r="563" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G563" s="51"/>
+      <c r="G563" s="48"/>
     </row>
     <row r="564" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G564" s="51"/>
+      <c r="G564" s="48"/>
     </row>
     <row r="565" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G565" s="51"/>
+      <c r="G565" s="48"/>
     </row>
     <row r="566" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G566" s="51"/>
+      <c r="G566" s="48"/>
     </row>
     <row r="567" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G567" s="51"/>
+      <c r="G567" s="48"/>
     </row>
     <row r="568" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G568" s="51"/>
+      <c r="G568" s="48"/>
     </row>
     <row r="569" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G569" s="51"/>
+      <c r="G569" s="48"/>
     </row>
     <row r="570" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G570" s="51"/>
+      <c r="G570" s="48"/>
     </row>
     <row r="571" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G571" s="51"/>
+      <c r="G571" s="48"/>
     </row>
     <row r="572" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G572" s="51"/>
+      <c r="G572" s="48"/>
     </row>
     <row r="573" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G573" s="51"/>
+      <c r="G573" s="48"/>
     </row>
     <row r="574" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G574" s="51"/>
+      <c r="G574" s="48"/>
     </row>
     <row r="575" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G575" s="51"/>
+      <c r="G575" s="48"/>
     </row>
     <row r="576" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G576" s="51"/>
+      <c r="G576" s="48"/>
     </row>
     <row r="577" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G577" s="51"/>
+      <c r="G577" s="48"/>
     </row>
     <row r="578" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G578" s="51"/>
+      <c r="G578" s="48"/>
     </row>
     <row r="579" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G579" s="51"/>
+      <c r="G579" s="48"/>
     </row>
     <row r="580" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G580" s="51"/>
+      <c r="G580" s="48"/>
     </row>
     <row r="581" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G581" s="51"/>
+      <c r="G581" s="48"/>
     </row>
     <row r="582" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G582" s="51"/>
+      <c r="G582" s="48"/>
     </row>
     <row r="583" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G583" s="51"/>
+      <c r="G583" s="48"/>
     </row>
     <row r="584" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G584" s="51"/>
+      <c r="G584" s="48"/>
     </row>
     <row r="585" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G585" s="51"/>
+      <c r="G585" s="48"/>
     </row>
     <row r="586" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G586" s="51"/>
+      <c r="G586" s="48"/>
     </row>
     <row r="587" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G587" s="51"/>
+      <c r="G587" s="48"/>
     </row>
     <row r="588" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G588" s="51"/>
+      <c r="G588" s="48"/>
     </row>
     <row r="589" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G589" s="51"/>
+      <c r="G589" s="48"/>
     </row>
     <row r="590" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G590" s="51"/>
+      <c r="G590" s="48"/>
     </row>
     <row r="591" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G591" s="51"/>
+      <c r="G591" s="48"/>
     </row>
     <row r="592" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G592" s="51"/>
+      <c r="G592" s="48"/>
     </row>
     <row r="593" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G593" s="51"/>
+      <c r="G593" s="48"/>
     </row>
     <row r="594" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G594" s="51"/>
+      <c r="G594" s="48"/>
     </row>
     <row r="595" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G595" s="51"/>
+      <c r="G595" s="48"/>
     </row>
     <row r="596" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G596" s="51"/>
+      <c r="G596" s="48"/>
     </row>
     <row r="597" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G597" s="51"/>
+      <c r="G597" s="48"/>
     </row>
     <row r="598" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G598" s="51"/>
+      <c r="G598" s="48"/>
     </row>
     <row r="599" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G599" s="51"/>
+      <c r="G599" s="48"/>
     </row>
     <row r="600" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G600" s="51"/>
+      <c r="G600" s="48"/>
     </row>
     <row r="601" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G601" s="51"/>
+      <c r="G601" s="48"/>
     </row>
     <row r="602" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G602" s="51"/>
+      <c r="G602" s="48"/>
     </row>
     <row r="603" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G603" s="51"/>
+      <c r="G603" s="48"/>
     </row>
     <row r="604" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G604" s="51"/>
+      <c r="G604" s="48"/>
     </row>
     <row r="605" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G605" s="51"/>
+      <c r="G605" s="48"/>
     </row>
     <row r="606" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G606" s="51"/>
+      <c r="G606" s="48"/>
     </row>
     <row r="607" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G607" s="51"/>
+      <c r="G607" s="48"/>
     </row>
     <row r="608" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G608" s="51"/>
+      <c r="G608" s="48"/>
     </row>
     <row r="609" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G609" s="51"/>
+      <c r="G609" s="48"/>
     </row>
     <row r="610" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G610" s="51"/>
+      <c r="G610" s="48"/>
     </row>
     <row r="611" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G611" s="51"/>
+      <c r="G611" s="48"/>
     </row>
     <row r="612" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G612" s="51"/>
+      <c r="G612" s="48"/>
     </row>
     <row r="613" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G613" s="51"/>
+      <c r="G613" s="48"/>
     </row>
     <row r="614" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G614" s="51"/>
+      <c r="G614" s="48"/>
     </row>
     <row r="615" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G615" s="51"/>
+      <c r="G615" s="48"/>
     </row>
     <row r="616" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G616" s="51"/>
+      <c r="G616" s="48"/>
     </row>
     <row r="617" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G617" s="51"/>
+      <c r="G617" s="48"/>
     </row>
     <row r="618" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G618" s="51"/>
+      <c r="G618" s="48"/>
     </row>
     <row r="619" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G619" s="51"/>
+      <c r="G619" s="48"/>
     </row>
     <row r="620" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G620" s="51"/>
+      <c r="G620" s="48"/>
     </row>
     <row r="621" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G621" s="51"/>
+      <c r="G621" s="48"/>
     </row>
     <row r="622" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G622" s="51"/>
+      <c r="G622" s="48"/>
     </row>
     <row r="623" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G623" s="51"/>
+      <c r="G623" s="48"/>
     </row>
     <row r="624" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G624" s="51"/>
+      <c r="G624" s="48"/>
     </row>
     <row r="625" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G625" s="51"/>
+      <c r="G625" s="48"/>
     </row>
     <row r="626" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G626" s="51"/>
+      <c r="G626" s="48"/>
     </row>
     <row r="627" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G627" s="51"/>
+      <c r="G627" s="48"/>
     </row>
     <row r="628" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G628" s="51"/>
+      <c r="G628" s="48"/>
     </row>
     <row r="629" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G629" s="51"/>
+      <c r="G629" s="48"/>
     </row>
     <row r="630" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G630" s="51"/>
+      <c r="G630" s="48"/>
     </row>
     <row r="631" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G631" s="51"/>
+      <c r="G631" s="48"/>
     </row>
     <row r="632" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G632" s="51"/>
+      <c r="G632" s="48"/>
     </row>
     <row r="633" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G633" s="51"/>
+      <c r="G633" s="48"/>
     </row>
     <row r="634" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G634" s="51"/>
+      <c r="G634" s="48"/>
     </row>
     <row r="635" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G635" s="51"/>
+      <c r="G635" s="48"/>
     </row>
     <row r="636" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G636" s="51"/>
+      <c r="G636" s="48"/>
     </row>
     <row r="637" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G637" s="51"/>
+      <c r="G637" s="48"/>
     </row>
     <row r="638" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G638" s="51"/>
+      <c r="G638" s="48"/>
     </row>
     <row r="639" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G639" s="51"/>
+      <c r="G639" s="48"/>
     </row>
     <row r="640" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G640" s="51"/>
+      <c r="G640" s="48"/>
     </row>
     <row r="641" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G641" s="51"/>
+      <c r="G641" s="48"/>
     </row>
     <row r="642" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G642" s="51"/>
+      <c r="G642" s="48"/>
     </row>
     <row r="643" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G643" s="51"/>
+      <c r="G643" s="48"/>
     </row>
     <row r="644" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G644" s="51"/>
+      <c r="G644" s="48"/>
     </row>
     <row r="645" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G645" s="51"/>
+      <c r="G645" s="48"/>
     </row>
     <row r="646" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G646" s="51"/>
+      <c r="G646" s="48"/>
     </row>
     <row r="647" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G647" s="51"/>
+      <c r="G647" s="48"/>
     </row>
     <row r="648" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G648" s="51"/>
+      <c r="G648" s="48"/>
     </row>
     <row r="649" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G649" s="51"/>
+      <c r="G649" s="48"/>
     </row>
     <row r="650" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G650" s="51"/>
+      <c r="G650" s="48"/>
     </row>
     <row r="651" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G651" s="51"/>
+      <c r="G651" s="48"/>
     </row>
     <row r="652" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G652" s="51"/>
+      <c r="G652" s="48"/>
     </row>
     <row r="653" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G653" s="51"/>
+      <c r="G653" s="48"/>
     </row>
     <row r="654" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G654" s="51"/>
+      <c r="G654" s="48"/>
     </row>
     <row r="655" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G655" s="51"/>
+      <c r="G655" s="48"/>
     </row>
     <row r="656" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G656" s="51"/>
+      <c r="G656" s="48"/>
     </row>
     <row r="657" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G657" s="51"/>
+      <c r="G657" s="48"/>
     </row>
     <row r="658" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G658" s="51"/>
+      <c r="G658" s="48"/>
     </row>
     <row r="659" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G659" s="51"/>
+      <c r="G659" s="48"/>
     </row>
     <row r="660" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G660" s="51"/>
+      <c r="G660" s="48"/>
     </row>
     <row r="661" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G661" s="51"/>
+      <c r="G661" s="48"/>
     </row>
     <row r="662" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G662" s="51"/>
+      <c r="G662" s="48"/>
     </row>
     <row r="663" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G663" s="51"/>
+      <c r="G663" s="48"/>
     </row>
     <row r="664" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G664" s="51"/>
+      <c r="G664" s="48"/>
     </row>
     <row r="665" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G665" s="51"/>
+      <c r="G665" s="48"/>
     </row>
     <row r="666" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G666" s="51"/>
+      <c r="G666" s="48"/>
     </row>
     <row r="667" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G667" s="51"/>
+      <c r="G667" s="48"/>
     </row>
     <row r="668" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G668" s="51"/>
+      <c r="G668" s="48"/>
     </row>
     <row r="669" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G669" s="51"/>
+      <c r="G669" s="48"/>
     </row>
     <row r="670" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G670" s="51"/>
+      <c r="G670" s="48"/>
     </row>
     <row r="671" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G671" s="51"/>
+      <c r="G671" s="48"/>
     </row>
     <row r="672" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G672" s="51"/>
+      <c r="G672" s="48"/>
     </row>
     <row r="673" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G673" s="51"/>
+      <c r="G673" s="48"/>
     </row>
     <row r="674" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G674" s="51"/>
+      <c r="G674" s="48"/>
     </row>
     <row r="675" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G675" s="51"/>
+      <c r="G675" s="48"/>
     </row>
     <row r="676" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G676" s="51"/>
+      <c r="G676" s="48"/>
     </row>
     <row r="677" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G677" s="51"/>
+      <c r="G677" s="48"/>
     </row>
     <row r="678" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G678" s="51"/>
+      <c r="G678" s="48"/>
     </row>
     <row r="679" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G679" s="51"/>
+      <c r="G679" s="48"/>
     </row>
     <row r="680" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G680" s="51"/>
+      <c r="G680" s="48"/>
     </row>
     <row r="681" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G681" s="51"/>
+      <c r="G681" s="48"/>
     </row>
     <row r="682" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G682" s="51"/>
+      <c r="G682" s="48"/>
     </row>
     <row r="683" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G683" s="51"/>
+      <c r="G683" s="48"/>
     </row>
     <row r="684" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G684" s="51"/>
+      <c r="G684" s="48"/>
     </row>
     <row r="685" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G685" s="51"/>
+      <c r="G685" s="48"/>
     </row>
     <row r="686" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G686" s="51"/>
+      <c r="G686" s="48"/>
     </row>
     <row r="687" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G687" s="51"/>
+      <c r="G687" s="48"/>
     </row>
     <row r="688" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G688" s="51"/>
+      <c r="G688" s="48"/>
     </row>
     <row r="689" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G689" s="51"/>
+      <c r="G689" s="48"/>
     </row>
     <row r="690" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G690" s="51"/>
+      <c r="G690" s="48"/>
     </row>
     <row r="691" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G691" s="51"/>
+      <c r="G691" s="48"/>
     </row>
     <row r="692" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G692" s="51"/>
+      <c r="G692" s="48"/>
     </row>
     <row r="693" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G693" s="51"/>
+      <c r="G693" s="48"/>
     </row>
     <row r="694" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G694" s="51"/>
+      <c r="G694" s="48"/>
     </row>
     <row r="695" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G695" s="51"/>
+      <c r="G695" s="48"/>
     </row>
     <row r="696" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G696" s="51"/>
+      <c r="G696" s="48"/>
     </row>
     <row r="697" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G697" s="51"/>
+      <c r="G697" s="48"/>
     </row>
     <row r="698" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G698" s="51"/>
+      <c r="G698" s="48"/>
     </row>
     <row r="699" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G699" s="51"/>
+      <c r="G699" s="48"/>
     </row>
     <row r="700" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G700" s="51"/>
+      <c r="G700" s="48"/>
     </row>
     <row r="701" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G701" s="51"/>
+      <c r="G701" s="48"/>
     </row>
     <row r="702" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G702" s="51"/>
+      <c r="G702" s="48"/>
     </row>
     <row r="703" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G703" s="51"/>
+      <c r="G703" s="48"/>
     </row>
     <row r="704" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G704" s="51"/>
+      <c r="G704" s="48"/>
     </row>
     <row r="705" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G705" s="51"/>
+      <c r="G705" s="48"/>
     </row>
     <row r="706" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G706" s="51"/>
+      <c r="G706" s="48"/>
     </row>
     <row r="707" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G707" s="51"/>
+      <c r="G707" s="48"/>
     </row>
     <row r="708" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G708" s="51"/>
+      <c r="G708" s="48"/>
     </row>
     <row r="709" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G709" s="51"/>
+      <c r="G709" s="48"/>
     </row>
     <row r="710" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G710" s="51"/>
+      <c r="G710" s="48"/>
     </row>
     <row r="711" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G711" s="51"/>
+      <c r="G711" s="48"/>
     </row>
     <row r="712" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G712" s="51"/>
+      <c r="G712" s="48"/>
     </row>
     <row r="713" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G713" s="51"/>
+      <c r="G713" s="48"/>
     </row>
     <row r="714" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G714" s="51"/>
+      <c r="G714" s="48"/>
     </row>
     <row r="715" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G715" s="51"/>
+      <c r="G715" s="48"/>
     </row>
     <row r="716" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G716" s="51"/>
+      <c r="G716" s="48"/>
     </row>
     <row r="717" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G717" s="51"/>
+      <c r="G717" s="48"/>
     </row>
     <row r="718" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G718" s="51"/>
+      <c r="G718" s="48"/>
     </row>
     <row r="719" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G719" s="51"/>
+      <c r="G719" s="48"/>
     </row>
     <row r="720" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G720" s="51"/>
+      <c r="G720" s="48"/>
     </row>
     <row r="721" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G721" s="51"/>
+      <c r="G721" s="48"/>
     </row>
     <row r="722" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G722" s="51"/>
+      <c r="G722" s="48"/>
     </row>
     <row r="723" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G723" s="51"/>
+      <c r="G723" s="48"/>
     </row>
     <row r="724" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G724" s="51"/>
+      <c r="G724" s="48"/>
     </row>
     <row r="725" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G725" s="51"/>
+      <c r="G725" s="48"/>
     </row>
     <row r="726" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G726" s="51"/>
+      <c r="G726" s="48"/>
     </row>
     <row r="727" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G727" s="51"/>
+      <c r="G727" s="48"/>
     </row>
     <row r="728" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G728" s="51"/>
+      <c r="G728" s="48"/>
     </row>
     <row r="729" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G729" s="51"/>
+      <c r="G729" s="48"/>
     </row>
     <row r="730" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G730" s="51"/>
+      <c r="G730" s="48"/>
     </row>
     <row r="731" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G731" s="51"/>
+      <c r="G731" s="48"/>
     </row>
     <row r="732" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G732" s="51"/>
+      <c r="G732" s="48"/>
     </row>
     <row r="733" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G733" s="51"/>
+      <c r="G733" s="48"/>
     </row>
     <row r="734" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G734" s="51"/>
+      <c r="G734" s="48"/>
     </row>
     <row r="735" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G735" s="51"/>
+      <c r="G735" s="48"/>
     </row>
     <row r="736" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G736" s="51"/>
+      <c r="G736" s="48"/>
     </row>
     <row r="737" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G737" s="51"/>
+      <c r="G737" s="48"/>
     </row>
     <row r="738" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G738" s="51"/>
+      <c r="G738" s="48"/>
     </row>
     <row r="739" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G739" s="51"/>
+      <c r="G739" s="48"/>
     </row>
     <row r="740" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G740" s="51"/>
+      <c r="G740" s="48"/>
     </row>
     <row r="741" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G741" s="51"/>
+      <c r="G741" s="48"/>
     </row>
     <row r="742" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G742" s="51"/>
+      <c r="G742" s="48"/>
     </row>
     <row r="743" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G743" s="51"/>
+      <c r="G743" s="48"/>
     </row>
     <row r="744" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G744" s="51"/>
+      <c r="G744" s="48"/>
     </row>
     <row r="745" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G745" s="51"/>
+      <c r="G745" s="48"/>
     </row>
     <row r="746" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G746" s="51"/>
+      <c r="G746" s="48"/>
     </row>
     <row r="747" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G747" s="51"/>
+      <c r="G747" s="48"/>
     </row>
     <row r="748" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G748" s="51"/>
+      <c r="G748" s="48"/>
     </row>
     <row r="749" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G749" s="51"/>
+      <c r="G749" s="48"/>
     </row>
     <row r="750" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G750" s="51"/>
+      <c r="G750" s="48"/>
     </row>
     <row r="751" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G751" s="51"/>
+      <c r="G751" s="48"/>
     </row>
     <row r="752" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G752" s="51"/>
+      <c r="G752" s="48"/>
     </row>
     <row r="753" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G753" s="51"/>
+      <c r="G753" s="48"/>
     </row>
     <row r="754" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G754" s="51"/>
+      <c r="G754" s="48"/>
     </row>
     <row r="755" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G755" s="51"/>
+      <c r="G755" s="48"/>
     </row>
     <row r="756" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G756" s="51"/>
+      <c r="G756" s="48"/>
     </row>
     <row r="757" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G757" s="51"/>
+      <c r="G757" s="48"/>
     </row>
     <row r="758" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G758" s="51"/>
+      <c r="G758" s="48"/>
     </row>
     <row r="759" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G759" s="51"/>
+      <c r="G759" s="48"/>
     </row>
     <row r="760" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G760" s="51"/>
+      <c r="G760" s="48"/>
     </row>
     <row r="761" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G761" s="51"/>
+      <c r="G761" s="48"/>
     </row>
     <row r="762" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G762" s="51"/>
+      <c r="G762" s="48"/>
     </row>
     <row r="763" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G763" s="51"/>
+      <c r="G763" s="48"/>
     </row>
     <row r="764" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G764" s="51"/>
+      <c r="G764" s="48"/>
     </row>
     <row r="765" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G765" s="51"/>
+      <c r="G765" s="48"/>
     </row>
     <row r="766" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G766" s="51"/>
+      <c r="G766" s="48"/>
     </row>
     <row r="767" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G767" s="51"/>
+      <c r="G767" s="48"/>
     </row>
     <row r="768" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G768" s="51"/>
+      <c r="G768" s="48"/>
     </row>
     <row r="769" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G769" s="51"/>
+      <c r="G769" s="48"/>
     </row>
     <row r="770" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G770" s="51"/>
+      <c r="G770" s="48"/>
     </row>
     <row r="771" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G771" s="51"/>
+      <c r="G771" s="48"/>
     </row>
     <row r="772" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G772" s="51"/>
+      <c r="G772" s="48"/>
     </row>
     <row r="773" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G773" s="51"/>
+      <c r="G773" s="48"/>
     </row>
     <row r="774" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G774" s="51"/>
+      <c r="G774" s="48"/>
     </row>
     <row r="775" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G775" s="51"/>
+      <c r="G775" s="48"/>
     </row>
     <row r="776" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G776" s="51"/>
+      <c r="G776" s="48"/>
     </row>
     <row r="777" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G777" s="51"/>
+      <c r="G777" s="48"/>
     </row>
     <row r="778" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G778" s="51"/>
+      <c r="G778" s="48"/>
     </row>
     <row r="779" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G779" s="51"/>
+      <c r="G779" s="48"/>
     </row>
     <row r="780" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G780" s="51"/>
+      <c r="G780" s="48"/>
     </row>
     <row r="781" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G781" s="51"/>
+      <c r="G781" s="48"/>
     </row>
     <row r="782" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G782" s="51"/>
+      <c r="G782" s="48"/>
     </row>
     <row r="783" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G783" s="51"/>
+      <c r="G783" s="48"/>
     </row>
     <row r="784" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G784" s="51"/>
+      <c r="G784" s="48"/>
     </row>
     <row r="785" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G785" s="51"/>
+      <c r="G785" s="48"/>
     </row>
     <row r="786" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G786" s="51"/>
+      <c r="G786" s="48"/>
     </row>
     <row r="787" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G787" s="51"/>
+      <c r="G787" s="48"/>
     </row>
     <row r="788" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G788" s="51"/>
+      <c r="G788" s="48"/>
     </row>
     <row r="789" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G789" s="51"/>
+      <c r="G789" s="48"/>
     </row>
     <row r="790" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G790" s="51"/>
+      <c r="G790" s="48"/>
     </row>
     <row r="791" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G791" s="51"/>
+      <c r="G791" s="48"/>
     </row>
     <row r="792" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G792" s="51"/>
+      <c r="G792" s="48"/>
     </row>
     <row r="793" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G793" s="51"/>
+      <c r="G793" s="48"/>
     </row>
     <row r="794" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G794" s="51"/>
+      <c r="G794" s="48"/>
     </row>
     <row r="795" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G795" s="51"/>
+      <c r="G795" s="48"/>
     </row>
     <row r="796" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G796" s="51"/>
+      <c r="G796" s="48"/>
     </row>
     <row r="797" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G797" s="51"/>
+      <c r="G797" s="48"/>
     </row>
     <row r="798" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G798" s="51"/>
+      <c r="G798" s="48"/>
     </row>
     <row r="799" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G799" s="51"/>
+      <c r="G799" s="48"/>
     </row>
     <row r="800" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G800" s="51"/>
+      <c r="G800" s="48"/>
     </row>
     <row r="801" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G801" s="51"/>
+      <c r="G801" s="48"/>
     </row>
     <row r="802" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G802" s="51"/>
+      <c r="G802" s="48"/>
     </row>
     <row r="803" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G803" s="51"/>
+      <c r="G803" s="48"/>
     </row>
     <row r="804" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G804" s="51"/>
+      <c r="G804" s="48"/>
     </row>
     <row r="805" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G805" s="51"/>
+      <c r="G805" s="48"/>
     </row>
     <row r="806" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G806" s="51"/>
+      <c r="G806" s="48"/>
     </row>
     <row r="807" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G807" s="51"/>
+      <c r="G807" s="48"/>
     </row>
     <row r="808" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G808" s="51"/>
+      <c r="G808" s="48"/>
     </row>
     <row r="809" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G809" s="51"/>
+      <c r="G809" s="48"/>
     </row>
     <row r="810" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G810" s="51"/>
+      <c r="G810" s="48"/>
     </row>
     <row r="811" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G811" s="51"/>
+      <c r="G811" s="48"/>
     </row>
     <row r="812" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G812" s="51"/>
+      <c r="G812" s="48"/>
     </row>
     <row r="813" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G813" s="51"/>
+      <c r="G813" s="48"/>
     </row>
     <row r="814" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G814" s="51"/>
+      <c r="G814" s="48"/>
     </row>
     <row r="815" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G815" s="51"/>
+      <c r="G815" s="48"/>
     </row>
     <row r="816" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G816" s="51"/>
+      <c r="G816" s="48"/>
     </row>
     <row r="817" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G817" s="51"/>
+      <c r="G817" s="48"/>
     </row>
     <row r="818" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G818" s="51"/>
+      <c r="G818" s="48"/>
     </row>
     <row r="819" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G819" s="51"/>
+      <c r="G819" s="48"/>
     </row>
     <row r="820" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G820" s="51"/>
+      <c r="G820" s="48"/>
     </row>
     <row r="821" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G821" s="51"/>
+      <c r="G821" s="48"/>
     </row>
     <row r="822" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G822" s="51"/>
+      <c r="G822" s="48"/>
     </row>
     <row r="823" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G823" s="51"/>
+      <c r="G823" s="48"/>
     </row>
     <row r="824" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G824" s="51"/>
+      <c r="G824" s="48"/>
     </row>
     <row r="825" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G825" s="51"/>
+      <c r="G825" s="48"/>
     </row>
     <row r="826" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G826" s="51"/>
+      <c r="G826" s="48"/>
     </row>
     <row r="827" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G827" s="51"/>
+      <c r="G827" s="48"/>
     </row>
     <row r="828" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G828" s="51"/>
+      <c r="G828" s="48"/>
     </row>
     <row r="829" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G829" s="51"/>
+      <c r="G829" s="48"/>
     </row>
     <row r="830" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G830" s="51"/>
+      <c r="G830" s="48"/>
     </row>
     <row r="831" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G831" s="51"/>
+      <c r="G831" s="48"/>
     </row>
     <row r="832" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G832" s="51"/>
+      <c r="G832" s="48"/>
     </row>
     <row r="833" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G833" s="51"/>
+      <c r="G833" s="48"/>
     </row>
     <row r="834" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G834" s="51"/>
+      <c r="G834" s="48"/>
     </row>
     <row r="835" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G835" s="51"/>
+      <c r="G835" s="48"/>
     </row>
     <row r="836" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G836" s="51"/>
+      <c r="G836" s="48"/>
     </row>
     <row r="837" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G837" s="51"/>
+      <c r="G837" s="48"/>
     </row>
     <row r="838" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G838" s="51"/>
+      <c r="G838" s="48"/>
     </row>
     <row r="839" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G839" s="51"/>
+      <c r="G839" s="48"/>
     </row>
     <row r="840" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G840" s="51"/>
+      <c r="G840" s="48"/>
     </row>
     <row r="841" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G841" s="51"/>
+      <c r="G841" s="48"/>
     </row>
     <row r="842" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G842" s="51"/>
+      <c r="G842" s="48"/>
     </row>
     <row r="843" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G843" s="51"/>
+      <c r="G843" s="48"/>
     </row>
     <row r="844" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G844" s="51"/>
+      <c r="G844" s="48"/>
     </row>
     <row r="845" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G845" s="51"/>
+      <c r="G845" s="48"/>
     </row>
     <row r="846" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G846" s="51"/>
+      <c r="G846" s="48"/>
     </row>
     <row r="847" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G847" s="51"/>
+      <c r="G847" s="48"/>
     </row>
     <row r="848" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G848" s="51"/>
+      <c r="G848" s="48"/>
     </row>
     <row r="849" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G849" s="51"/>
+      <c r="G849" s="48"/>
     </row>
     <row r="850" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G850" s="51"/>
+      <c r="G850" s="48"/>
     </row>
     <row r="851" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G851" s="51"/>
+      <c r="G851" s="48"/>
     </row>
     <row r="852" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G852" s="51"/>
+      <c r="G852" s="48"/>
     </row>
     <row r="853" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G853" s="51"/>
+      <c r="G853" s="48"/>
     </row>
     <row r="854" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G854" s="51"/>
+      <c r="G854" s="48"/>
     </row>
     <row r="855" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G855" s="51"/>
+      <c r="G855" s="48"/>
     </row>
     <row r="856" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G856" s="51"/>
+      <c r="G856" s="48"/>
     </row>
     <row r="857" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G857" s="51"/>
+      <c r="G857" s="48"/>
     </row>
     <row r="858" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G858" s="51"/>
+      <c r="G858" s="48"/>
     </row>
     <row r="859" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G859" s="51"/>
+      <c r="G859" s="48"/>
     </row>
     <row r="860" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G860" s="51"/>
+      <c r="G860" s="48"/>
     </row>
     <row r="861" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G861" s="51"/>
+      <c r="G861" s="48"/>
     </row>
     <row r="862" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G862" s="51"/>
+      <c r="G862" s="48"/>
     </row>
     <row r="863" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G863" s="51"/>
+      <c r="G863" s="48"/>
     </row>
     <row r="864" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G864" s="51"/>
+      <c r="G864" s="48"/>
     </row>
     <row r="865" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G865" s="51"/>
+      <c r="G865" s="48"/>
     </row>
     <row r="866" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G866" s="51"/>
+      <c r="G866" s="48"/>
     </row>
     <row r="867" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G867" s="51"/>
+      <c r="G867" s="48"/>
     </row>
     <row r="868" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G868" s="51"/>
+      <c r="G868" s="48"/>
     </row>
     <row r="869" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G869" s="51"/>
+      <c r="G869" s="48"/>
     </row>
     <row r="870" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G870" s="51"/>
+      <c r="G870" s="48"/>
     </row>
     <row r="871" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G871" s="51"/>
+      <c r="G871" s="48"/>
     </row>
     <row r="872" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G872" s="51"/>
+      <c r="G872" s="48"/>
     </row>
     <row r="873" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G873" s="51"/>
+      <c r="G873" s="48"/>
     </row>
     <row r="874" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G874" s="51"/>
+      <c r="G874" s="48"/>
     </row>
     <row r="875" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G875" s="51"/>
+      <c r="G875" s="48"/>
     </row>
     <row r="876" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G876" s="51"/>
+      <c r="G876" s="48"/>
     </row>
     <row r="877" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G877" s="51"/>
+      <c r="G877" s="48"/>
     </row>
     <row r="878" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G878" s="51"/>
+      <c r="G878" s="48"/>
     </row>
     <row r="879" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G879" s="51"/>
+      <c r="G879" s="48"/>
     </row>
     <row r="880" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G880" s="51"/>
+      <c r="G880" s="48"/>
     </row>
     <row r="881" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G881" s="51"/>
+      <c r="G881" s="48"/>
     </row>
     <row r="882" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G882" s="51"/>
+      <c r="G882" s="48"/>
     </row>
     <row r="883" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G883" s="51"/>
+      <c r="G883" s="48"/>
     </row>
     <row r="884" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G884" s="51"/>
+      <c r="G884" s="48"/>
     </row>
     <row r="885" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G885" s="51"/>
+      <c r="G885" s="48"/>
     </row>
     <row r="886" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G886" s="51"/>
+      <c r="G886" s="48"/>
     </row>
     <row r="887" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G887" s="51"/>
+      <c r="G887" s="48"/>
     </row>
     <row r="888" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G888" s="51"/>
+      <c r="G888" s="48"/>
     </row>
     <row r="889" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G889" s="51"/>
+      <c r="G889" s="48"/>
     </row>
     <row r="890" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G890" s="51"/>
+      <c r="G890" s="48"/>
     </row>
     <row r="891" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G891" s="51"/>
+      <c r="G891" s="48"/>
     </row>
     <row r="892" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G892" s="51"/>
+      <c r="G892" s="48"/>
     </row>
     <row r="893" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G893" s="51"/>
+      <c r="G893" s="48"/>
     </row>
     <row r="894" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G894" s="51"/>
+      <c r="G894" s="48"/>
     </row>
     <row r="895" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G895" s="51"/>
+      <c r="G895" s="48"/>
     </row>
     <row r="896" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G896" s="51"/>
+      <c r="G896" s="48"/>
     </row>
     <row r="897" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G897" s="51"/>
+      <c r="G897" s="48"/>
     </row>
     <row r="898" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G898" s="51"/>
+      <c r="G898" s="48"/>
     </row>
     <row r="899" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G899" s="51"/>
+      <c r="G899" s="48"/>
     </row>
     <row r="900" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G900" s="51"/>
+      <c r="G900" s="48"/>
     </row>
     <row r="901" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G901" s="51"/>
+      <c r="G901" s="48"/>
     </row>
     <row r="902" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G902" s="51"/>
+      <c r="G902" s="48"/>
     </row>
     <row r="903" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G903" s="51"/>
+      <c r="G903" s="48"/>
     </row>
     <row r="904" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G904" s="51"/>
+      <c r="G904" s="48"/>
     </row>
     <row r="905" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G905" s="51"/>
+      <c r="G905" s="48"/>
     </row>
     <row r="906" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G906" s="51"/>
+      <c r="G906" s="48"/>
     </row>
     <row r="907" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G907" s="51"/>
+      <c r="G907" s="48"/>
     </row>
     <row r="908" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G908" s="51"/>
+      <c r="G908" s="48"/>
     </row>
     <row r="909" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G909" s="51"/>
+      <c r="G909" s="48"/>
     </row>
     <row r="910" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G910" s="51"/>
+      <c r="G910" s="48"/>
     </row>
     <row r="911" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G911" s="51"/>
+      <c r="G911" s="48"/>
     </row>
     <row r="912" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G912" s="51"/>
+      <c r="G912" s="48"/>
     </row>
     <row r="913" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G913" s="51"/>
+      <c r="G913" s="48"/>
     </row>
     <row r="914" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G914" s="51"/>
+      <c r="G914" s="48"/>
     </row>
     <row r="915" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G915" s="51"/>
+      <c r="G915" s="48"/>
     </row>
     <row r="916" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G916" s="51"/>
+      <c r="G916" s="48"/>
     </row>
     <row r="917" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G917" s="51"/>
+      <c r="G917" s="48"/>
     </row>
     <row r="918" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G918" s="51"/>
+      <c r="G918" s="48"/>
     </row>
     <row r="919" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G919" s="51"/>
+      <c r="G919" s="48"/>
     </row>
     <row r="920" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G920" s="51"/>
+      <c r="G920" s="48"/>
     </row>
     <row r="921" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G921" s="51"/>
+      <c r="G921" s="48"/>
     </row>
     <row r="922" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G922" s="51"/>
+      <c r="G922" s="48"/>
     </row>
     <row r="923" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G923" s="51"/>
+      <c r="G923" s="48"/>
     </row>
     <row r="924" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G924" s="51"/>
+      <c r="G924" s="48"/>
     </row>
     <row r="925" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G925" s="51"/>
+      <c r="G925" s="48"/>
     </row>
     <row r="926" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G926" s="51"/>
+      <c r="G926" s="48"/>
     </row>
     <row r="927" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G927" s="51"/>
+      <c r="G927" s="48"/>
     </row>
     <row r="928" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G928" s="51"/>
+      <c r="G928" s="48"/>
     </row>
     <row r="929" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G929" s="51"/>
+      <c r="G929" s="48"/>
     </row>
     <row r="930" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G930" s="51"/>
+      <c r="G930" s="48"/>
     </row>
     <row r="931" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G931" s="51"/>
+      <c r="G931" s="48"/>
     </row>
     <row r="932" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G932" s="51"/>
+      <c r="G932" s="48"/>
     </row>
     <row r="933" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G933" s="51"/>
+      <c r="G933" s="48"/>
     </row>
     <row r="934" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G934" s="51"/>
+      <c r="G934" s="48"/>
     </row>
     <row r="935" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G935" s="51"/>
+      <c r="G935" s="48"/>
     </row>
     <row r="936" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G936" s="51"/>
+      <c r="G936" s="48"/>
     </row>
     <row r="937" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G937" s="51"/>
+      <c r="G937" s="48"/>
     </row>
     <row r="938" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G938" s="51"/>
+      <c r="G938" s="48"/>
     </row>
     <row r="939" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G939" s="51"/>
+      <c r="G939" s="48"/>
     </row>
     <row r="940" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G940" s="51"/>
+      <c r="G940" s="48"/>
     </row>
     <row r="941" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G941" s="51"/>
+      <c r="G941" s="48"/>
     </row>
     <row r="942" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G942" s="51"/>
+      <c r="G942" s="48"/>
     </row>
     <row r="943" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G943" s="51"/>
+      <c r="G943" s="48"/>
     </row>
     <row r="944" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G944" s="51"/>
+      <c r="G944" s="48"/>
     </row>
     <row r="945" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G945" s="51"/>
+      <c r="G945" s="48"/>
     </row>
     <row r="946" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G946" s="51"/>
+      <c r="G946" s="48"/>
     </row>
     <row r="947" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G947" s="51"/>
+      <c r="G947" s="48"/>
     </row>
     <row r="948" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G948" s="51"/>
+      <c r="G948" s="48"/>
     </row>
     <row r="949" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G949" s="51"/>
+      <c r="G949" s="48"/>
     </row>
     <row r="950" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G950" s="51"/>
+      <c r="G950" s="48"/>
     </row>
     <row r="951" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G951" s="51"/>
+      <c r="G951" s="48"/>
     </row>
     <row r="952" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G952" s="51"/>
+      <c r="G952" s="48"/>
     </row>
     <row r="953" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G953" s="51"/>
+      <c r="G953" s="48"/>
     </row>
     <row r="954" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G954" s="51"/>
+      <c r="G954" s="48"/>
     </row>
     <row r="955" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G955" s="51"/>
+      <c r="G955" s="48"/>
     </row>
     <row r="956" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G956" s="51"/>
+      <c r="G956" s="48"/>
     </row>
     <row r="957" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G957" s="51"/>
+      <c r="G957" s="48"/>
     </row>
     <row r="958" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G958" s="51"/>
+      <c r="G958" s="48"/>
     </row>
     <row r="959" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G959" s="51"/>
+      <c r="G959" s="48"/>
     </row>
     <row r="960" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G960" s="51"/>
+      <c r="G960" s="48"/>
     </row>
     <row r="961" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G961" s="51"/>
+      <c r="G961" s="48"/>
     </row>
     <row r="962" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G962" s="51"/>
+      <c r="G962" s="48"/>
     </row>
     <row r="963" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G963" s="51"/>
+      <c r="G963" s="48"/>
     </row>
     <row r="964" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G964" s="51"/>
+      <c r="G964" s="48"/>
     </row>
     <row r="965" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G965" s="51"/>
+      <c r="G965" s="48"/>
     </row>
     <row r="966" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G966" s="51"/>
+      <c r="G966" s="48"/>
     </row>
     <row r="967" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G967" s="51"/>
+      <c r="G967" s="48"/>
     </row>
     <row r="968" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G968" s="51"/>
+      <c r="G968" s="48"/>
     </row>
     <row r="969" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G969" s="51"/>
+      <c r="G969" s="48"/>
     </row>
     <row r="970" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G970" s="51"/>
+      <c r="G970" s="48"/>
     </row>
     <row r="971" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G971" s="51"/>
+      <c r="G971" s="48"/>
     </row>
     <row r="972" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G972" s="51"/>
+      <c r="G972" s="48"/>
     </row>
     <row r="973" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G973" s="51"/>
+      <c r="G973" s="48"/>
     </row>
     <row r="974" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G974" s="51"/>
+      <c r="G974" s="48"/>
     </row>
     <row r="975" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G975" s="51"/>
+      <c r="G975" s="48"/>
     </row>
     <row r="976" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G976" s="51"/>
+      <c r="G976" s="48"/>
     </row>
     <row r="977" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G977" s="51"/>
+      <c r="G977" s="48"/>
     </row>
     <row r="978" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G978" s="51"/>
+      <c r="G978" s="48"/>
     </row>
     <row r="979" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G979" s="51"/>
+      <c r="G979" s="48"/>
     </row>
     <row r="980" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G980" s="51"/>
+      <c r="G980" s="48"/>
     </row>
     <row r="981" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G981" s="51"/>
+      <c r="G981" s="48"/>
     </row>
     <row r="982" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G982" s="51"/>
+      <c r="G982" s="48"/>
     </row>
     <row r="983" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G983" s="51"/>
+      <c r="G983" s="48"/>
     </row>
     <row r="984" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G984" s="51"/>
+      <c r="G984" s="48"/>
     </row>
     <row r="985" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G985" s="51"/>
+      <c r="G985" s="48"/>
     </row>
     <row r="986" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G986" s="51"/>
+      <c r="G986" s="48"/>
     </row>
     <row r="987" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G987" s="51"/>
+      <c r="G987" s="48"/>
     </row>
     <row r="988" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G988" s="51"/>
+      <c r="G988" s="48"/>
     </row>
     <row r="989" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G989" s="51"/>
+      <c r="G989" s="48"/>
     </row>
     <row r="990" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G990" s="51"/>
+      <c r="G990" s="48"/>
     </row>
     <row r="991" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G991" s="51"/>
+      <c r="G991" s="48"/>
     </row>
     <row r="992" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G992" s="51"/>
+      <c r="G992" s="48"/>
     </row>
     <row r="993" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G993" s="51"/>
+      <c r="G993" s="48"/>
     </row>
     <row r="994" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G994" s="51"/>
+      <c r="G994" s="48"/>
     </row>
     <row r="995" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G995" s="51"/>
+      <c r="G995" s="48"/>
     </row>
     <row r="996" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G996" s="51"/>
+      <c r="G996" s="48"/>
     </row>
     <row r="997" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G997" s="51"/>
+      <c r="G997" s="48"/>
     </row>
     <row r="998" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G998" s="51"/>
+      <c r="G998" s="48"/>
     </row>
     <row r="999" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G999" s="51"/>
+      <c r="G999" s="48"/>
     </row>
     <row r="1000" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G1000" s="51"/>
+      <c r="G1000" s="48"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -74924,6 +74950,8 @@
     <hyperlink ref="D7" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
     <hyperlink ref="F7" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
     <hyperlink ref="D3" r:id="rId18" xr:uid="{B834FDED-B3E1-7949-91B7-96E51068AF9E}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{E246F9AA-64FE-6F40-B89D-866BF4BE9028}"/>
+    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{0759FAAD-CF5A-2E46-ADC1-192E07CD0B77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Add "local sequence file" option for data source
</commit_message>
<xml_diff>
--- a/package template.xlsx
+++ b/package template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAD901-DE52-FF44-8A54-8328496CED01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB5EA5C-24F1-0D44-8E64-DB9B22ED14E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="800" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7552" uniqueCount="7521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7555" uniqueCount="7524">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22657,6 +22657,15 @@
   </si>
   <si>
     <t>{REPLACE_HERE}</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Local Sequence File</t>
+  </si>
+  <si>
+    <t>Local : mRFP1a</t>
   </si>
 </sst>
 </file>
@@ -23009,7 +23018,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23071,6 +23080,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23527,7 +23537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -71728,8 +71738,8 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -71903,14 +71913,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="22" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" s="42" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>7517</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>7517</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="46" t="s">
         <v>7518</v>
       </c>
@@ -71920,17 +71930,26 @@
       <c r="F8" s="52" t="s">
         <v>7520</v>
       </c>
-      <c r="G8" s="48" t="b">
+      <c r="G8" s="53" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="G9" s="48"/>
+    <row r="9" spans="1:7" s="42" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="15" t="s">
+        <v>7521</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>7522</v>
+      </c>
+      <c r="C9" s="52"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="15" t="s">
+        <v>7523</v>
+      </c>
+      <c r="F9" s="52"/>
+      <c r="G9" s="53" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
@@ -74950,8 +74969,8 @@
     <hyperlink ref="D7" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
     <hyperlink ref="F7" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
     <hyperlink ref="D3" r:id="rId18" xr:uid="{B834FDED-B3E1-7949-91B7-96E51068AF9E}"/>
-    <hyperlink ref="D8" r:id="rId19" xr:uid="{E246F9AA-64FE-6F40-B89D-866BF4BE9028}"/>
-    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{0759FAAD-CF5A-2E46-ADC1-192E07CD0B77}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{5C6F1B5E-BBD2-284F-81B8-F83B79F659F2}"/>
+    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{215768AB-C316-6346-A526-B19A764F7251}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
added a utility to make it easier to propagate changes from the template to other packages; applied it to copy the updated data_source sheet into the packages
</commit_message>
<xml_diff>
--- a/package template.xlsx
+++ b/package template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB5EA5C-24F1-0D44-8E64-DB9B22ED14E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8839388A-4515-B14B-8F0E-17491B6D0416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23537,8 +23537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -71738,7 +71738,7 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Support for imports from any URL retrieving a GenBank or FASTA file Also renames "GenBank_imports" to "NCBI_GenBank_imports" vs. "Other_GenBank_imports" Upgrade to use of next sbol-utilities alpha
</commit_message>
<xml_diff>
--- a/package template.xlsx
+++ b/package template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8839388A-4515-B14B-8F0E-17491B6D0416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745E8F08-2772-0C4B-96F3-0A88717B9E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1360" windowWidth="34060" windowHeight="19800" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7555" uniqueCount="7524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7565" uniqueCount="7532">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22638,9 +22638,6 @@
     <t>Template Version:</t>
   </si>
   <si>
-    <t>1.0a2</t>
-  </si>
-  <si>
     <t>DNA Parts and Devices</t>
   </si>
   <si>
@@ -22665,7 +22662,34 @@
     <t>Local Sequence File</t>
   </si>
   <si>
-    <t>Local : mRFP1a</t>
+    <t>1.0a3</t>
+  </si>
+  <si>
+    <t>ExtGB</t>
+  </si>
+  <si>
+    <t>ExtFA</t>
+  </si>
+  <si>
+    <t>Local: mRFP1a</t>
+  </si>
+  <si>
+    <t>ExtGB: https://freegenes.github.io/genbank/BBF10K_003338.gb</t>
+  </si>
+  <si>
+    <t>ExtFA: http://parts.igem.org/cgi/partsdb/composite_edit/putseq.cgi?part=BBa_J23101</t>
+  </si>
+  <si>
+    <t>URL for FASTA file</t>
+  </si>
+  <si>
+    <t>URL for GenBank file</t>
+  </si>
+  <si>
+    <t>https://freegenes.github.io/genbank/BBF10K_003338.gb</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/iGEM-Engineering/iGEM-distribution/develop/scripts/test/test_files/BBa_J23101.fasta</t>
   </si>
 </sst>
 </file>
@@ -23074,13 +23098,13 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23537,7 +23561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -23608,12 +23632,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -23758,7 +23782,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>7515</v>
+        <v>7514</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>13</v>
@@ -71738,8 +71762,8 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -71772,7 +71796,7 @@
         <v>7467</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>7516</v>
+        <v>7515</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -71915,57 +71939,83 @@
     </row>
     <row r="8" spans="1:7" s="42" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
+        <v>7516</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>7516</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="46" t="s">
         <v>7517</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>7517</v>
-      </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="46" t="s">
+      <c r="E8" s="15" t="s">
         <v>7518</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="49" t="s">
         <v>7519</v>
       </c>
-      <c r="F8" s="52" t="s">
-        <v>7520</v>
-      </c>
-      <c r="G8" s="53" t="b">
+      <c r="G8" s="50" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="42" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="15" t="s">
+        <v>7520</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>7521</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>7522</v>
-      </c>
-      <c r="C9" s="52"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="46"/>
       <c r="E9" s="15" t="s">
+        <v>7525</v>
+      </c>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="42" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="15" t="s">
         <v>7523</v>
       </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="G10" s="48"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="48"/>
+      <c r="B10" s="15" t="s">
+        <v>7529</v>
+      </c>
+      <c r="C10" s="49"/>
+      <c r="D10" s="46" t="s">
+        <v>7530</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>7526</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>7519</v>
+      </c>
+      <c r="G10" s="50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="42" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A11" s="15" t="s">
+        <v>7524</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>7528</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="46" t="s">
+        <v>7531</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>7527</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>7519</v>
+      </c>
+      <c r="G11" s="50" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
@@ -74971,6 +75021,10 @@
     <hyperlink ref="D3" r:id="rId18" xr:uid="{B834FDED-B3E1-7949-91B7-96E51068AF9E}"/>
     <hyperlink ref="D8" r:id="rId19" xr:uid="{5C6F1B5E-BBD2-284F-81B8-F83B79F659F2}"/>
     <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{215768AB-C316-6346-A526-B19A764F7251}"/>
+    <hyperlink ref="F10" r:id="rId21" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{2C064FF4-DFD6-274F-9927-F751C315AA95}"/>
+    <hyperlink ref="F11" r:id="rId22" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{96A88FBD-5684-3245-A20C-456252846DDA}"/>
+    <hyperlink ref="D10" r:id="rId23" xr:uid="{D2139E6E-0A23-9C4B-9528-7D3047A573DC}"/>
+    <hyperlink ref="D11" r:id="rId24" xr:uid="{9426E70A-F730-B141-BFD4-EF0AD05C4729}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -74984,9 +75038,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -74999,7 +75051,7 @@
         <v>7513</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>7514</v>
+        <v>7522</v>
       </c>
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>

</xml_diff>